<commit_message>
changes in test Plan
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/SalesOrder_BaseData_SOAPI.xlsx
+++ b/templates/AutomationOrg/SalesOrder_BaseData_SOAPI.xlsx
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="201">
   <si>
     <t>Customer</t>
   </si>
@@ -632,6 +632,39 @@
   </si>
   <si>
     <t>99414.0</t>
+  </si>
+  <si>
+    <t>94.0</t>
+  </si>
+  <si>
+    <t>97802.0</t>
+  </si>
+  <si>
+    <t>98901.0</t>
+  </si>
+  <si>
+    <t>93.0</t>
+  </si>
+  <si>
+    <t>97800.0</t>
+  </si>
+  <si>
+    <t>98900.0</t>
+  </si>
+  <si>
+    <t>92.0</t>
+  </si>
+  <si>
+    <t>97798.0</t>
+  </si>
+  <si>
+    <t>98899.0</t>
+  </si>
+  <si>
+    <t>97796.0</t>
+  </si>
+  <si>
+    <t>98898.0</t>
   </si>
 </sst>
 </file>
@@ -641,7 +674,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="181" x14ac:knownFonts="1">
+  <fonts count="217" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -686,6 +719,222 @@
       <color rgb="FF202124"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -1740,7 +1989,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="88">
+  <borders count="106">
     <border>
       <left/>
       <right/>
@@ -2009,11 +2258,65 @@
     <border>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="184">
+  <cellXfs count="220">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
@@ -2198,8 +2501,44 @@
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="85" fillId="0" fontId="176" numFmtId="49" xfId="0"/>
     <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="177" numFmtId="164" xfId="0"/>
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="86" fillId="0" fontId="178" numFmtId="49" xfId="0"/>
-    <xf numFmtId="164" fontId="179" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="180" fillId="0" borderId="87" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="179" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="87" fillId="0" fontId="180" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="181" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="88" fillId="0" fontId="182" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="183" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="89" fillId="0" fontId="184" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="185" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="90" fillId="0" fontId="186" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="187" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="91" fillId="0" fontId="188" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="189" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="92" fillId="0" fontId="190" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="191" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="93" fillId="0" fontId="192" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="193" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="94" fillId="0" fontId="194" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="195" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="95" fillId="0" fontId="196" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="197" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="96" fillId="0" fontId="198" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="199" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="97" fillId="0" fontId="200" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="201" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="98" fillId="0" fontId="202" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="203" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="99" fillId="0" fontId="204" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="205" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="100" fillId="0" fontId="206" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="207" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="101" fillId="0" fontId="208" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="209" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="102" fillId="0" fontId="210" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="211" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="103" fillId="0" fontId="212" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="213" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="104" fillId="0" fontId="214" numFmtId="49" xfId="0"/>
+    <xf numFmtId="164" fontId="215" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="216" fillId="0" borderId="105" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -4722,7 +5061,7 @@
         <v>126</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>188</v>
+        <v>199</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>165</v>
@@ -4736,7 +5075,7 @@
         <v>70</v>
       </c>
       <c r="B4" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="C4" t="s">
         <v>166</v>

</xml_diff>

<commit_message>
Project Sync and added/Updated testplans
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/SalesOrder_BaseData_SOAPI.xlsx
+++ b/templates/AutomationOrg/SalesOrder_BaseData_SOAPI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok\Provar\RSTK_Automation\rsqasampleproj\templates\AutomationOrg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{3AEE612F-D20D-4380-B129-7863B454B0FA}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{349E109C-6687-4857-9F49-5867572EC020}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView activeTab="3" firstSheet="15" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView activeTab="3" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="AddHeader" r:id="rId1" sheetId="14"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="172">
   <si>
     <t>Customer</t>
   </si>
@@ -494,60 +494,6 @@
     <t>DiscountPct</t>
   </si>
   <si>
-    <t>71.0</t>
-  </si>
-  <si>
-    <t>97406.0</t>
-  </si>
-  <si>
-    <t>98702.0</t>
-  </si>
-  <si>
-    <t>69.0</t>
-  </si>
-  <si>
-    <t>97402.0</t>
-  </si>
-  <si>
-    <t>98700.0</t>
-  </si>
-  <si>
-    <t>70.0</t>
-  </si>
-  <si>
-    <t>97404.0</t>
-  </si>
-  <si>
-    <t>98701.0</t>
-  </si>
-  <si>
-    <t>68.0</t>
-  </si>
-  <si>
-    <t>97400.0</t>
-  </si>
-  <si>
-    <t>98699.0</t>
-  </si>
-  <si>
-    <t>67.0</t>
-  </si>
-  <si>
-    <t>97398.0</t>
-  </si>
-  <si>
-    <t>98698.0</t>
-  </si>
-  <si>
-    <t>75.0</t>
-  </si>
-  <si>
-    <t>97313.0</t>
-  </si>
-  <si>
-    <t>98656.0</t>
-  </si>
-  <si>
     <t>74.0</t>
   </si>
   <si>
@@ -555,6 +501,84 @@
   </si>
   <si>
     <t>98655.0</t>
+  </si>
+  <si>
+    <t>39.0</t>
+  </si>
+  <si>
+    <t>97241.0</t>
+  </si>
+  <si>
+    <t>98620.0</t>
+  </si>
+  <si>
+    <t>38.0</t>
+  </si>
+  <si>
+    <t>97239.0</t>
+  </si>
+  <si>
+    <t>98619.0</t>
+  </si>
+  <si>
+    <t>36.0</t>
+  </si>
+  <si>
+    <t>97235.0</t>
+  </si>
+  <si>
+    <t>98617.0</t>
+  </si>
+  <si>
+    <t>37.0</t>
+  </si>
+  <si>
+    <t>97237.0</t>
+  </si>
+  <si>
+    <t>98618.0</t>
+  </si>
+  <si>
+    <t>35.0</t>
+  </si>
+  <si>
+    <t>97233.0</t>
+  </si>
+  <si>
+    <t>98616.0</t>
+  </si>
+  <si>
+    <t>135.0</t>
+  </si>
+  <si>
+    <t>97232.0</t>
+  </si>
+  <si>
+    <t>134.0</t>
+  </si>
+  <si>
+    <t>97230.0</t>
+  </si>
+  <si>
+    <t>98615.0</t>
+  </si>
+  <si>
+    <t>133.0</t>
+  </si>
+  <si>
+    <t>97228.0</t>
+  </si>
+  <si>
+    <t>98614.0</t>
+  </si>
+  <si>
+    <t>132.0</t>
+  </si>
+  <si>
+    <t>97226.0</t>
+  </si>
+  <si>
+    <t>98613.0</t>
   </si>
 </sst>
 </file>
@@ -564,7 +588,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="79" x14ac:knownFonts="1">
+  <fonts count="85" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -609,6 +633,42 @@
       <color rgb="FF202124"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -1051,7 +1111,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="37">
+  <borders count="40">
     <border>
       <left/>
       <right/>
@@ -1167,11 +1227,20 @@
     <border>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="88">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
@@ -1254,8 +1323,14 @@
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="34" fillId="0" fontId="74" numFmtId="49" xfId="0"/>
     <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="75" numFmtId="164" xfId="0"/>
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="35" fillId="0" fontId="76" numFmtId="49" xfId="0"/>
-    <xf numFmtId="164" fontId="77" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="78" fillId="0" borderId="36" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="77" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="36" fillId="0" fontId="78" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="79" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="37" fillId="0" fontId="80" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="81" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="38" fillId="0" fontId="82" numFmtId="49" xfId="0"/>
+    <xf numFmtId="164" fontId="83" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="84" fillId="0" borderId="39" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -2198,8 +2273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8EBB0E8-7736-4B3E-8E32-A499FC9E511B}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2266,7 +2341,7 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="H1" sqref="H1:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3396,10 +3471,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F745D4BD-94B9-4920-AF2D-A59E170DB0E2}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3410,14 +3485,15 @@
     <col min="5" max="5" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -3440,22 +3516,25 @@
         <v>1</v>
       </c>
       <c r="H1" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="I1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>43</v>
       </c>
@@ -3477,23 +3556,26 @@
       <c r="G2" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2">
         <v>2</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>200</v>
       </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2" t="b">
-        <v>1</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="b">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>43</v>
       </c>
@@ -3515,20 +3597,23 @@
       <c r="G3" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="H3">
+      <c r="H3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3">
         <v>4</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>100</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>2</v>
       </c>
-      <c r="K3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>43</v>
       </c>
@@ -3550,20 +3635,23 @@
       <c r="G4" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="H4">
+      <c r="H4" t="s">
+        <v>49</v>
+      </c>
+      <c r="I4">
         <v>2</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>50</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>3</v>
       </c>
-      <c r="K4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>43</v>
       </c>
@@ -3585,20 +3673,23 @@
       <c r="G5" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I5">
         <v>2</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>80</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>4</v>
       </c>
-      <c r="K5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>43</v>
       </c>
@@ -3620,16 +3711,19 @@
       <c r="G6" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I6">
         <v>3</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>20</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>5</v>
       </c>
-      <c r="K6" t="b">
+      <c r="L6" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3831,10 +3925,10 @@
         <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="C2" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -3845,10 +3939,10 @@
         <v>126</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -3859,10 +3953,10 @@
         <v>70</v>
       </c>
       <c r="B4" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="C4" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="D4">
         <v>1</v>

</xml_diff>